<commit_message>
Fixing excel file from 2016-03-23
</commit_message>
<xml_diff>
--- a/results/2016-03-23/Summary.xlsx
+++ b/results/2016-03-23/Summary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>Platform</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>After load</t>
+  </si>
+  <si>
+    <t>Ratio vs Best (WS)</t>
+  </si>
+  <si>
+    <t>Ratio vs Best (PB)</t>
   </si>
 </sst>
 </file>
@@ -114,17 +120,30 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -218,7 +237,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$13</c:f>
+              <c:f>Sheet1!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -239,7 +258,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$14:$A$20</c:f>
+              <c:f>Sheet1!$H$3:$H$9</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -268,7 +287,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$B$20</c:f>
+              <c:f>Sheet1!$I$3:$I$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -307,7 +326,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$13</c:f>
+              <c:f>Sheet1!$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -328,7 +347,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$14:$A$20</c:f>
+              <c:f>Sheet1!$H$3:$H$9</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -357,7 +376,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$14:$C$20</c:f>
+              <c:f>Sheet1!$J$3:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -396,7 +415,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$13</c:f>
+              <c:f>Sheet1!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -417,7 +436,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$14:$A$20</c:f>
+              <c:f>Sheet1!$H$3:$H$9</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -446,7 +465,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$14:$D$20</c:f>
+              <c:f>Sheet1!$K$3:$K$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2305,16 +2324,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57710</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>33057</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>202826</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>99732</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2335,16 +2354,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>164167</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>401171</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>49867</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2367,26 +2386,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:D9" totalsRowShown="0">
-  <autoFilter ref="A2:D9"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:F9" totalsRowShown="0">
+  <autoFilter ref="A2:F9"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Platform"/>
     <tableColumn id="2" name="Committed"/>
     <tableColumn id="3" name="Private Bytes"/>
     <tableColumn id="4" name="Working Set"/>
+    <tableColumn id="5" name="Ratio vs Best (WS)" dataDxfId="3">
+      <calculatedColumnFormula>ROUND(D3/MIN(D$3:D$9),1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Ratio vs Best (PB)" dataDxfId="1">
+      <calculatedColumnFormula>ROUND(C3/MIN(C$3:C$9),1)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A13:D20" totalsRowShown="0">
-  <autoFilter ref="A13:D20"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="H2:M9" totalsRowShown="0">
+  <autoFilter ref="H2:M9"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Platform"/>
     <tableColumn id="2" name="Committed"/>
     <tableColumn id="3" name="Private Bytes"/>
     <tableColumn id="4" name="Working Set"/>
+    <tableColumn id="5" name="Ratio vs Best (WS)" dataDxfId="2">
+      <calculatedColumnFormula>ROUND(K3/MIN(K$3:K$9),1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Ratio vs Best (PB)" dataDxfId="0">
+      <calculatedColumnFormula>ROUND(J3/MIN(J$3:J$9),1)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2689,11 +2720,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2701,20 +2730,30 @@
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="6" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2727,8 +2766,32 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2741,8 +2804,36 @@
       <c r="D3">
         <v>27404</v>
       </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E9" si="0">ROUND(D3/MIN(D$3:D$9),1)</f>
+        <v>1.8</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F9" si="1">ROUND(C3/MIN(C$3:C$9),1)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>143728</v>
+      </c>
+      <c r="J3">
+        <v>75660</v>
+      </c>
+      <c r="K3">
+        <v>97588</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L9" si="2">ROUND(K3/MIN(K$3:K$9),1)</f>
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M9" si="3">ROUND(J3/MIN(J$3:J$9),1)</f>
+        <v>2.7</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2755,8 +2846,36 @@
       <c r="D4">
         <v>31652</v>
       </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>1.7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>217560</v>
+      </c>
+      <c r="J4">
+        <v>73760</v>
+      </c>
+      <c r="K4">
+        <v>94040</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>2.9</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="3"/>
+        <v>2.6</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2769,8 +2888,36 @@
       <c r="D5">
         <v>15120</v>
       </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>61852</v>
+      </c>
+      <c r="J5">
+        <v>27932</v>
+      </c>
+      <c r="K5">
+        <v>32748</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2783,8 +2930,36 @@
       <c r="D6">
         <v>20864</v>
       </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6">
+        <v>69276</v>
+      </c>
+      <c r="J6">
+        <v>35356</v>
+      </c>
+      <c r="K6">
+        <v>37772</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="3"/>
+        <v>1.3</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2797,8 +2972,36 @@
       <c r="D7">
         <v>397280</v>
       </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>26.3</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>42.8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <v>646764</v>
+      </c>
+      <c r="J7">
+        <v>573212</v>
+      </c>
+      <c r="K7">
+        <v>462748</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>14.1</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="3"/>
+        <v>20.5</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2811,8 +3014,36 @@
       <c r="D8">
         <v>40340</v>
       </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>2.7</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>36.4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8">
+        <v>931528</v>
+      </c>
+      <c r="J8">
+        <v>864456</v>
+      </c>
+      <c r="K8">
+        <v>523540</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>30.9</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2825,128 +3056,81 @@
       <c r="D9">
         <v>128588</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14">
-        <v>143728</v>
-      </c>
-      <c r="C14">
-        <v>75660</v>
-      </c>
-      <c r="D14">
-        <v>97588</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15">
-        <v>217560</v>
-      </c>
-      <c r="C15">
-        <v>73760</v>
-      </c>
-      <c r="D15">
-        <v>94040</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16">
-        <v>61852</v>
-      </c>
-      <c r="C16">
-        <v>27932</v>
-      </c>
-      <c r="D16">
-        <v>32748</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17">
-        <v>69276</v>
-      </c>
-      <c r="C17">
-        <v>35356</v>
-      </c>
-      <c r="D17">
-        <v>37772</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18">
-        <v>646764</v>
-      </c>
-      <c r="C18">
-        <v>573212</v>
-      </c>
-      <c r="D18">
-        <v>462748</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19">
-        <v>931528</v>
-      </c>
-      <c r="C19">
-        <v>864456</v>
-      </c>
-      <c r="D19">
-        <v>523540</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>41.8</v>
+      </c>
+      <c r="H9" t="s">
         <v>10</v>
       </c>
-      <c r="B20">
+      <c r="I9">
         <v>600296</v>
       </c>
-      <c r="C20">
+      <c r="J9">
         <v>533628</v>
       </c>
-      <c r="D20">
+      <c r="K9">
         <v>136436</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>4.2</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>19.100000000000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E1:G1"/>
   </mergeCells>
+  <conditionalFormatting sqref="E3:F9">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0FB5BBA0-6A78-440F-847D-7D72C925E3DD}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L9">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{35C32F9C-3AA2-48A9-BC2B-E7794A58704B}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M9">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{B100C088-9AB4-4A00-AB09-779BAFBD3021}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2954,5 +3138,50 @@
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0FB5BBA0-6A78-440F-847D-7D72C925E3DD}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E3:F9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{35C32F9C-3AA2-48A9-BC2B-E7794A58704B}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L3:L9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B100C088-9AB4-4A00-AB09-779BAFBD3021}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M3:M9</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>